<commit_message>
Fixed the command line issue in CQLReplicator-calculator.xlsx
</commit_message>
<xml_diff>
--- a/glue/resources/CQLReplicator-calculator.xlsx
+++ b/glue/resources/CQLReplicator-calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kolesnn/IdeaProjects/cql-replicator/glue/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BD74EB-2F44-9142-9D5E-D7C12DEAF3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E58E59-6D1F-144D-A30D-9E2B40F7E9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="58380" windowHeight="25260" xr2:uid="{E1F5BCB3-0904-F044-A203-C0CE43AF672C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{E1F5BCB3-0904-F044-A203-C0CE43AF672C}"/>
   </bookViews>
   <sheets>
     <sheet name="List of artifacts" sheetId="1" r:id="rId1"/>
@@ -761,7 +761,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -853,8 +853,8 @@
         <v>29</v>
       </c>
       <c r="E2" s="6" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G2),"$WORKER_TYPE",H2),"$SRC_KS",D2),"$SRC_TBL",A2),"$TRG_KS",D2),"$TRG_TBL",D2),"$WC",K2), " --orw ", R2), "--writetime-column N/A", "")</f>
-        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 9 --worker-type G.025X --src-keyspace my_keyspace --src-table my_table1 --trg-keyspace my_keyspace --trg-table my_keyspace --writetime-column col1 --json-mapping '{
+        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G2),"$WORKER_TYPE",H2),"$SRC_KS",D2),"$SRC_TBL",A2),"$TRG_KS",D2),"$TRG_TBL",A2),"$WC",K2), " --orw ", R2), "--writetime-column N/A", "")</f>
+        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 9 --worker-type G.025X --src-keyspace my_keyspace --src-table my_table1 --trg-keyspace my_keyspace --trg-table my_table1 --writetime-column col1 --json-mapping '{
     "replication": {
         "useMaterializedView": {
             "enabled": true,
@@ -928,8 +928,8 @@
         <v>29</v>
       </c>
       <c r="E3" s="6" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G3),"$WORKER_TYPE",H3),"$SRC_KS",D3),"$SRC_TBL",A3),"$TRG_KS",D3),"$TRG_TBL",D3),"$WC",K3), " --orw ", R3), "--writetime-column N/A", "")</f>
-        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 6 --worker-type G.025X --src-keyspace my_keyspace --src-table my_table2 --trg-keyspace my_keyspace --trg-table my_keyspace --writetime-column col3 --json-mapping '{
+        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G3),"$WORKER_TYPE",H3),"$SRC_KS",D3),"$SRC_TBL",A3),"$TRG_KS",D3),"$TRG_TBL",A3),"$WC",K3), " --orw ", R3), "--writetime-column N/A", "")</f>
+        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 6 --worker-type G.025X --src-keyspace my_keyspace --src-table my_table2 --trg-keyspace my_keyspace --trg-table my_table2 --writetime-column col3 --json-mapping '{
     "replication": {
         "useMaterializedView": {
             "enabled": true,
@@ -1003,8 +1003,8 @@
         <v>29</v>
       </c>
       <c r="E4" s="6" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G4),"$WORKER_TYPE",H4),"$SRC_KS",D4),"$SRC_TBL",A4),"$TRG_KS",D4),"$TRG_TBL",D4),"$WC",K4), " --orw ", R4), "--writetime-column N/A", "")</f>
-        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 1 --worker-type G.1X --src-keyspace my_keyspace --src-table my_table3 --trg-keyspace my_keyspace --trg-table my_keyspace --writetime-column col4 --json-mapping '{
+        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G4),"$WORKER_TYPE",H4),"$SRC_KS",D4),"$SRC_TBL",A4),"$TRG_KS",D4),"$TRG_TBL",A4),"$WC",K4), " --orw ", R4), "--writetime-column N/A", "")</f>
+        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 1 --worker-type G.1X --src-keyspace my_keyspace --src-table my_table3 --trg-keyspace my_keyspace --trg-table my_table3 --writetime-column col4 --json-mapping '{
     "replication": {
         "useMaterializedView": {
             "enabled": true,
@@ -1078,8 +1078,8 @@
         <v>29</v>
       </c>
       <c r="E5" s="6" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G5),"$WORKER_TYPE",H5),"$SRC_KS",D5),"$SRC_TBL",A5),"$TRG_KS",D5),"$TRG_TBL",D5),"$WC",K5), " --orw ", R5), "--writetime-column N/A", "")</f>
-        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 1 --worker-type G.1X --src-keyspace my_keyspace --src-table my_table4 --trg-keyspace my_keyspace --trg-table my_keyspace  --json-mapping '{
+        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G5),"$WORKER_TYPE",H5),"$SRC_KS",D5),"$SRC_TBL",A5),"$TRG_KS",D5),"$TRG_TBL",A5),"$WC",K5), " --orw ", R5), "--writetime-column N/A", "")</f>
+        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 1 --worker-type G.1X --src-keyspace my_keyspace --src-table my_table4 --trg-keyspace my_keyspace --trg-table my_table4  --json-mapping '{
     "replication": {
         "useMaterializedView": {
             "enabled": true,
@@ -1153,8 +1153,8 @@
         <v>29</v>
       </c>
       <c r="E6" s="6" t="str">
-        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G6),"$WORKER_TYPE",H6),"$SRC_KS",D6),"$SRC_TBL",A6),"$TRG_KS",D6),"$TRG_TBL",D6),"$WC",K6), " --orw ", R6), "--writetime-column N/A", "")</f>
-        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 2 --worker-type G.2X --src-keyspace my_keyspace --src-table my_table4 --trg-keyspace my_keyspace --trg-table my_keyspace --writetime-column col5 --json-mapping '{
+        <f>SUBSTITUTE(_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Parameters!B$11,"$TILES",G6),"$WORKER_TYPE",H6),"$SRC_KS",D6),"$SRC_TBL",A6),"$TRG_KS",D6),"$TRG_TBL",A6),"$WC",K6), " --orw ", R6), "--writetime-column N/A", "")</f>
+        <v>./cqlreplicator --state run --inc-traffic --landing-zone s3://cql-replicator-eu-central-1 --region eu-central-1 --tiles 2 --worker-type G.2X --src-keyspace my_keyspace --src-table my_table4 --trg-keyspace my_keyspace --trg-table my_table4 --writetime-column col5 --json-mapping '{
     "replication": {
         "useMaterializedView": {
             "enabled": true,

</xml_diff>